<commit_message>
remade to calculate metrics
</commit_message>
<xml_diff>
--- a/Proteasome/in_vitro/const/results/5CV/external.xlsx
+++ b/Proteasome/in_vitro/const/results/5CV/external.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t>model</t>
   </si>
@@ -25,7 +25,25 @@
     <t>auc_roc</t>
   </si>
   <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Sens</t>
+  </si>
+  <si>
+    <t>Spec</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
     <t>ap</t>
+  </si>
+  <si>
+    <t>MCC</t>
   </si>
   <si>
     <t>const_2</t>
@@ -392,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,10 +429,28 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -423,12 +459,30 @@
         <v>0.668685689249957</v>
       </c>
       <c r="D2">
+        <v>-0.0248</v>
+      </c>
+      <c r="E2">
+        <v>0.6480811006517017</v>
+      </c>
+      <c r="F2">
+        <v>0.5918484500574053</v>
+      </c>
+      <c r="G2">
+        <v>0.6167146974063401</v>
+      </c>
+      <c r="H2">
+        <v>0.6199647753545534</v>
+      </c>
+      <c r="I2">
         <v>0.6127721186666475</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="J2">
+        <v>0.2384180296414633</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -437,12 +491,30 @@
         <v>0.6739960995080909</v>
       </c>
       <c r="D3">
+        <v>-0.0251</v>
+      </c>
+      <c r="E3">
+        <v>0.6502890173410405</v>
+      </c>
+      <c r="F3">
+        <v>0.5988538681948424</v>
+      </c>
+      <c r="G3">
+        <v>0.6216043464365612</v>
+      </c>
+      <c r="H3">
+        <v>0.6245714427679414</v>
+      </c>
+      <c r="I3">
         <v>0.6042867555550365</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="J3">
+        <v>0.2475429241065827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -451,12 +523,30 @@
         <v>0.6549033079545497</v>
       </c>
       <c r="D4">
+        <v>-0.0659</v>
+      </c>
+      <c r="E4">
+        <v>0.6679447852760736</v>
+      </c>
+      <c r="F4">
+        <v>0.5538648813146683</v>
+      </c>
+      <c r="G4">
+        <v>0.6043434000678656</v>
+      </c>
+      <c r="H4">
+        <v>0.6109048332953709</v>
+      </c>
+      <c r="I4">
         <v>0.6131068920318887</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="J4">
+        <v>0.2212064866901051</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -465,12 +555,30 @@
         <v>0.6756517382446958</v>
       </c>
       <c r="D5">
+        <v>-0.031</v>
+      </c>
+      <c r="E5">
+        <v>0.6560693641618497</v>
+      </c>
+      <c r="F5">
+        <v>0.6051575931232092</v>
+      </c>
+      <c r="G5">
+        <v>0.6276765739852989</v>
+      </c>
+      <c r="H5">
+        <v>0.6306134786425295</v>
+      </c>
+      <c r="I5">
         <v>0.5983399346707234</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="J5">
+        <v>0.2595385726506007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -479,12 +587,30 @@
         <v>0.6699813256703712</v>
       </c>
       <c r="D6">
+        <v>-0.0207</v>
+      </c>
+      <c r="E6">
+        <v>0.6510115606936416</v>
+      </c>
+      <c r="F6">
+        <v>0.6045845272206304</v>
+      </c>
+      <c r="G6">
+        <v>0.6251198465963567</v>
+      </c>
+      <c r="H6">
+        <v>0.627798043957136</v>
+      </c>
+      <c r="I6">
         <v>0.5786926109149777</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="J6">
+        <v>0.2539257275638001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -493,12 +619,30 @@
         <v>0.5737901199260635</v>
       </c>
       <c r="D7">
+        <v>0.1221</v>
+      </c>
+      <c r="E7">
+        <v>0.5162866449511401</v>
+      </c>
+      <c r="F7">
+        <v>0.6152356358941252</v>
+      </c>
+      <c r="G7">
+        <v>0.5714800144040332</v>
+      </c>
+      <c r="H7">
+        <v>0.5657611404226326</v>
+      </c>
+      <c r="I7">
         <v>0.4982295435028793</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="J7">
+        <v>0.1315002297077156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -507,12 +651,30 @@
         <v>0.6701030287161266</v>
       </c>
       <c r="D8">
+        <v>-0.0221</v>
+      </c>
+      <c r="E8">
+        <v>0.648121387283237</v>
+      </c>
+      <c r="F8">
+        <v>0.5946100917431193</v>
+      </c>
+      <c r="G8">
+        <v>0.6182864450127877</v>
+      </c>
+      <c r="H8">
+        <v>0.6213657395131782</v>
+      </c>
+      <c r="I8">
         <v>0.6108945196645301</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="J8">
+        <v>0.2411974555708757</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -521,12 +683,30 @@
         <v>0.6410621004201138</v>
       </c>
       <c r="D9">
+        <v>0.0011</v>
+      </c>
+      <c r="E9">
+        <v>0.6212700841622035</v>
+      </c>
+      <c r="F9">
+        <v>0.5990279465370595</v>
+      </c>
+      <c r="G9">
+        <v>0.6088723332204538</v>
+      </c>
+      <c r="H9">
+        <v>0.6101490153496315</v>
+      </c>
+      <c r="I9">
         <v>0.5619034754627009</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="J9">
+        <v>0.2188426121002955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -535,12 +715,30 @@
         <v>0.6280127136833068</v>
       </c>
       <c r="D10">
+        <v>-0.0045</v>
+      </c>
+      <c r="E10">
+        <v>0.6425081433224755</v>
+      </c>
+      <c r="F10">
+        <v>0.5419896640826873</v>
+      </c>
+      <c r="G10">
+        <v>0.5864553314121037</v>
+      </c>
+      <c r="H10">
+        <v>0.5922489037025814</v>
+      </c>
+      <c r="I10">
         <v>0.5911800841802024</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="J10">
+        <v>0.183846149044855</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -549,12 +747,30 @@
         <v>0.6038259602166388</v>
       </c>
       <c r="D11">
+        <v>-0.3597</v>
+      </c>
+      <c r="E11">
+        <v>0.7890173410404624</v>
+      </c>
+      <c r="F11">
+        <v>0.4</v>
+      </c>
+      <c r="G11">
+        <v>0.5720677532758069</v>
+      </c>
+      <c r="H11">
+        <v>0.5945086705202312</v>
+      </c>
+      <c r="I11">
         <v>0.516979016941902</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="J11">
+        <v>0.2018572817469966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -563,12 +779,30 @@
         <v>0.6670454260217671</v>
       </c>
       <c r="D12">
+        <v>-0.0424</v>
+      </c>
+      <c r="E12">
+        <v>0.6748278500382555</v>
+      </c>
+      <c r="F12">
+        <v>0.5795868772782503</v>
+      </c>
+      <c r="G12">
+        <v>0.6217406027768371</v>
+      </c>
+      <c r="H12">
+        <v>0.6272073636582529</v>
+      </c>
+      <c r="I12">
         <v>0.6082296602170314</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="J12">
+        <v>0.2532855768052678</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -577,12 +811,30 @@
         <v>0.6010571073488622</v>
       </c>
       <c r="D13">
+        <v>-0.0284</v>
+      </c>
+      <c r="E13">
+        <v>0.6050488599348535</v>
+      </c>
+      <c r="F13">
+        <v>0.5564880568108457</v>
+      </c>
+      <c r="G13">
+        <v>0.5779618293122074</v>
+      </c>
+      <c r="H13">
+        <v>0.5807684583728496</v>
+      </c>
+      <c r="I13">
         <v>0.5274190823687025</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="J13">
+        <v>0.1605258081251991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -591,12 +843,30 @@
         <v>0.6722672152850723</v>
       </c>
       <c r="D14">
+        <v>-0.09370000000000001</v>
+      </c>
+      <c r="E14">
+        <v>0.6789587852494577</v>
+      </c>
+      <c r="F14">
+        <v>0.566189111747851</v>
+      </c>
+      <c r="G14">
+        <v>0.6160485933503836</v>
+      </c>
+      <c r="H14">
+        <v>0.6225739484986543</v>
+      </c>
+      <c r="I14">
         <v>0.6084934568938282</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="J14">
+        <v>0.2443726198242345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -605,12 +875,30 @@
         <v>0.6177441326995379</v>
       </c>
       <c r="D15">
+        <v>-0.3172</v>
+      </c>
+      <c r="E15">
+        <v>0.7644508670520231</v>
+      </c>
+      <c r="F15">
+        <v>0.4320916905444126</v>
+      </c>
+      <c r="G15">
+        <v>0.5790987535953979</v>
+      </c>
+      <c r="H15">
+        <v>0.5982712787982178</v>
+      </c>
+      <c r="I15">
         <v>0.5285515278549074</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="J15">
+        <v>0.2053239010133639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -619,12 +907,30 @@
         <v>0.6608889789627029</v>
       </c>
       <c r="D16">
+        <v>-0.0143</v>
+      </c>
+      <c r="E16">
+        <v>0.6472838561591431</v>
+      </c>
+      <c r="F16">
+        <v>0.6087484811664642</v>
+      </c>
+      <c r="G16">
+        <v>0.625804266847274</v>
+      </c>
+      <c r="H16">
+        <v>0.6280161686628036</v>
+      </c>
+      <c r="I16">
         <v>0.5911971558175545</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="J16">
+        <v>0.2543502875078236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -633,12 +939,30 @@
         <v>0.6331165013167266</v>
       </c>
       <c r="D17">
+        <v>-0.1596</v>
+      </c>
+      <c r="E17">
+        <v>0.7008670520231214</v>
+      </c>
+      <c r="F17">
+        <v>0.5083094555873926</v>
+      </c>
+      <c r="G17">
+        <v>0.5934803451581975</v>
+      </c>
+      <c r="H17">
+        <v>0.6045882538052569</v>
+      </c>
+      <c r="I17">
         <v>0.5450426216124982</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="J17">
+        <v>0.2107909322208737</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -647,12 +971,30 @@
         <v>0.5857814119858772</v>
       </c>
       <c r="D18">
+        <v>0.0805</v>
+      </c>
+      <c r="E18">
+        <v>0.5374592833876222</v>
+      </c>
+      <c r="F18">
+        <v>0.6081342801807618</v>
+      </c>
+      <c r="G18">
+        <v>0.5768815268275117</v>
+      </c>
+      <c r="H18">
+        <v>0.5727967817841919</v>
+      </c>
+      <c r="I18">
         <v>0.5079147172131714</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="J18">
+        <v>0.1451744827080149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -661,12 +1003,30 @@
         <v>0.6207664185993697</v>
       </c>
       <c r="D19">
+        <v>0.0364</v>
+      </c>
+      <c r="E19">
+        <v>0.5944625407166124</v>
+      </c>
+      <c r="F19">
+        <v>0.5984506132989025</v>
+      </c>
+      <c r="G19">
+        <v>0.5966870723802665</v>
+      </c>
+      <c r="H19">
+        <v>0.5964565770077574</v>
+      </c>
+      <c r="I19">
         <v>0.555694601712853</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="J19">
+        <v>0.1916862476088877</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -675,12 +1035,30 @@
         <v>0.6598049943244201</v>
       </c>
       <c r="D20">
+        <v>-0.09</v>
+      </c>
+      <c r="E20">
+        <v>0.6916602907421576</v>
+      </c>
+      <c r="F20">
+        <v>0.5437424058323208</v>
+      </c>
+      <c r="G20">
+        <v>0.6092109718929902</v>
+      </c>
+      <c r="H20">
+        <v>0.6177013482872392</v>
+      </c>
+      <c r="I20">
         <v>0.6158775685020653</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="J20">
+        <v>0.2355742392936088</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -689,12 +1067,30 @@
         <v>0.5828829900870256</v>
       </c>
       <c r="D21">
+        <v>-0.1366</v>
+      </c>
+      <c r="E21">
+        <v>0.667176740627391</v>
+      </c>
+      <c r="F21">
+        <v>0.4896719319562576</v>
+      </c>
+      <c r="G21">
+        <v>0.5682356925160853</v>
+      </c>
+      <c r="H21">
+        <v>0.5784243362918242</v>
+      </c>
+      <c r="I21">
         <v>0.5006920722304524</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="J21">
+        <v>0.1578322638825122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B22">
         <v>9</v>
@@ -703,12 +1099,30 @@
         <v>0.6633239933399092</v>
       </c>
       <c r="D22">
+        <v>-0.0785</v>
+      </c>
+      <c r="E22">
+        <v>0.6916602907421576</v>
+      </c>
+      <c r="F22">
+        <v>0.5498177399756987</v>
+      </c>
+      <c r="G22">
+        <v>0.6125973586183542</v>
+      </c>
+      <c r="H22">
+        <v>0.6207390153589282</v>
+      </c>
+      <c r="I22">
         <v>0.6171196972237472</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="J22">
+        <v>0.2414590633205912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B23">
         <v>11</v>
@@ -717,12 +1131,30 @@
         <v>0.6570345993964745</v>
       </c>
       <c r="D23">
+        <v>-0.1014</v>
+      </c>
+      <c r="E23">
+        <v>0.6893649579188983</v>
+      </c>
+      <c r="F23">
+        <v>0.5364963503649635</v>
+      </c>
+      <c r="G23">
+        <v>0.6042019654354456</v>
+      </c>
+      <c r="H23">
+        <v>0.6129306541419308</v>
+      </c>
+      <c r="I23">
         <v>0.6148324542470879</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="J23">
+        <v>0.2262176485281562</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -731,12 +1163,30 @@
         <v>0.6272258580016741</v>
       </c>
       <c r="D24">
+        <v>0.0501</v>
+      </c>
+      <c r="E24">
+        <v>0.5890522875816994</v>
+      </c>
+      <c r="F24">
+        <v>0.5989650711513583</v>
+      </c>
+      <c r="G24">
+        <v>0.5945848375451264</v>
+      </c>
+      <c r="H24">
+        <v>0.5940086793665289</v>
+      </c>
+      <c r="I24">
         <v>0.5926368480001289</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="J24">
+        <v>0.1868370053756606</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -745,12 +1195,30 @@
         <v>0.6525274525067493</v>
       </c>
       <c r="D25">
+        <v>-0.0441</v>
+      </c>
+      <c r="E25">
+        <v>0.6567919075144508</v>
+      </c>
+      <c r="F25">
+        <v>0.5816618911174785</v>
+      </c>
+      <c r="G25">
+        <v>0.614892937040588</v>
+      </c>
+      <c r="H25">
+        <v>0.6192268993159646</v>
+      </c>
+      <c r="I25">
         <v>0.5629302006440207</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="J25">
+        <v>0.2371304879529483</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -759,12 +1227,30 @@
         <v>0.6763173476655018</v>
       </c>
       <c r="D26">
+        <v>-0.0801</v>
+      </c>
+      <c r="E26">
+        <v>0.6856936416184971</v>
+      </c>
+      <c r="F26">
+        <v>0.5822349570200573</v>
+      </c>
+      <c r="G26">
+        <v>0.6279961649089166</v>
+      </c>
+      <c r="H26">
+        <v>0.6339642993192772</v>
+      </c>
+      <c r="I26">
         <v>0.5906261796931629</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="J26">
+        <v>0.266842590931199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -773,12 +1259,30 @@
         <v>0.6289609982693468</v>
       </c>
       <c r="D27">
+        <v>0.0436</v>
+      </c>
+      <c r="E27">
+        <v>0.5985342019543974</v>
+      </c>
+      <c r="F27">
+        <v>0.591994835377663</v>
+      </c>
+      <c r="G27">
+        <v>0.5948865682391069</v>
+      </c>
+      <c r="H27">
+        <v>0.5952645186660301</v>
+      </c>
+      <c r="I27">
         <v>0.5882279846562506</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="J27">
+        <v>0.1892745628538845</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>7</v>
@@ -787,12 +1291,30 @@
         <v>0.6293166443413107</v>
       </c>
       <c r="D28">
+        <v>0.2278</v>
+      </c>
+      <c r="E28">
+        <v>0.4698697068403909</v>
+      </c>
+      <c r="F28">
+        <v>0.7198192382182053</v>
+      </c>
+      <c r="G28">
+        <v>0.6092906013683832</v>
+      </c>
+      <c r="H28">
+        <v>0.5948444725292981</v>
+      </c>
+      <c r="I28">
         <v>0.5754267868165599</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="J28">
+        <v>0.1957924704011453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -801,12 +1323,30 @@
         <v>0.6660574288739669</v>
       </c>
       <c r="D29">
+        <v>0.0342</v>
+      </c>
+      <c r="E29">
+        <v>0.6159143075745983</v>
+      </c>
+      <c r="F29">
+        <v>0.6233292831105711</v>
+      </c>
+      <c r="G29">
+        <v>0.6200474094141551</v>
+      </c>
+      <c r="H29">
+        <v>0.6196217953425847</v>
+      </c>
+      <c r="I29">
         <v>0.6151995379378776</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="J29">
+        <v>0.2378066044490126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -815,12 +1355,30 @@
         <v>0.5582402642873515</v>
       </c>
       <c r="D30">
+        <v>0.0254</v>
+      </c>
+      <c r="E30">
+        <v>0.5464169381107492</v>
+      </c>
+      <c r="F30">
+        <v>0.5506778566817302</v>
+      </c>
+      <c r="G30">
+        <v>0.5487936622254231</v>
+      </c>
+      <c r="H30">
+        <v>0.5485473973962397</v>
+      </c>
+      <c r="I30">
         <v>0.4871660170670571</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="J30">
+        <v>0.09645550671473291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -829,12 +1387,30 @@
         <v>0.6183500191974981</v>
       </c>
       <c r="D31">
+        <v>-0.1969</v>
+      </c>
+      <c r="E31">
+        <v>0.7061973986228003</v>
+      </c>
+      <c r="F31">
+        <v>0.4939246658566221</v>
+      </c>
+      <c r="G31">
+        <v>0.5878767355231967</v>
+      </c>
+      <c r="H31">
+        <v>0.6000610322397112</v>
+      </c>
+      <c r="I31">
         <v>0.5328322959755007</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="J31">
+        <v>0.2024595898483784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -843,12 +1419,30 @@
         <v>0.6296914790040017</v>
       </c>
       <c r="D32">
+        <v>0.06320000000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.5830618892508144</v>
+      </c>
+      <c r="F32">
+        <v>0.6120077469335055</v>
+      </c>
+      <c r="G32">
+        <v>0.5992077781778898</v>
+      </c>
+      <c r="H32">
+        <v>0.5975348180921599</v>
+      </c>
+      <c r="I32">
         <v>0.5836778284478448</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="J32">
+        <v>0.194019441855549</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -857,12 +1451,30 @@
         <v>0.6014115971481722</v>
       </c>
       <c r="D33">
+        <v>-0.1219</v>
+      </c>
+      <c r="E33">
+        <v>0.6641162968630452</v>
+      </c>
+      <c r="F33">
+        <v>0.5103280680437424</v>
+      </c>
+      <c r="G33">
+        <v>0.5783948526921775</v>
+      </c>
+      <c r="H33">
+        <v>0.5872221824533939</v>
+      </c>
+      <c r="I33">
         <v>0.5119925029970177</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="J33">
+        <v>0.1748624886989197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B34">
         <v>11</v>
@@ -871,7 +1483,25 @@
         <v>0.6275420939851917</v>
       </c>
       <c r="D34">
+        <v>0.0433</v>
+      </c>
+      <c r="E34">
+        <v>0.5944625407166124</v>
+      </c>
+      <c r="F34">
+        <v>0.591994835377663</v>
+      </c>
+      <c r="G34">
+        <v>0.5930860640979474</v>
+      </c>
+      <c r="H34">
+        <v>0.5932286880471377</v>
+      </c>
+      <c r="I34">
         <v>0.5922627625262181</v>
+      </c>
+      <c r="J34">
+        <v>0.1852412431697797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>